<commit_message>
Encoder Added, Silkscreen Updated, Bom Updated
</commit_message>
<xml_diff>
--- a/Hardware/Extra/Bottom/Smartwatch-EXTRA-BOTTOM_BOM.xlsx
+++ b/Hardware/Extra/Bottom/Smartwatch-EXTRA-BOTTOM_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruhaan Joshi\Documents\Smartwatch\Hardware\Basic\Bottom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruhaan Joshi\Documents\Smartwatch\Hardware\Extra\Bottom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486280CC-905C-4725-8C3F-7F52EB2A2613}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D69293D-C8CF-498D-BDF5-6C993993D843}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="14400" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6945" yWindow="3015" windowWidth="14400" windowHeight="11340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="146">
   <si>
     <t>BOM #</t>
   </si>
@@ -424,24 +424,6 @@
     <t>1727-2956-1-ND</t>
   </si>
   <si>
-    <t>NFET</t>
-  </si>
-  <si>
-    <t>N-Channel 30V 500mA (Ta) 690mW (Ta) Surface Mount SOT-23-3 (TO-236)</t>
-  </si>
-  <si>
-    <t>SOT23-3</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>NTR4003NT3G</t>
-  </si>
-  <si>
-    <t>NTR4003NT3GOSCT-ND</t>
-  </si>
-  <si>
     <t>CRYSTALECS-.327-12.5-12-C-TR (CRYSTAL) (32.7680kHz)</t>
   </si>
   <si>
@@ -583,9 +565,6 @@
     <t>1276-1274-1-ND</t>
   </si>
   <si>
-    <t>R1,R2,R7,R8,R14</t>
-  </si>
-  <si>
     <t>R10,R13</t>
   </si>
   <si>
@@ -625,12 +604,6 @@
     <t>C12</t>
   </si>
   <si>
-    <t>C5,C6,C7</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
     <t>AD5171</t>
   </si>
   <si>
@@ -652,7 +625,55 @@
     <t>XTAL1</t>
   </si>
   <si>
-    <t>J1</t>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>C5,C10</t>
+  </si>
+  <si>
+    <t>C6,C7</t>
+  </si>
+  <si>
+    <t>10 nF capacitor</t>
+  </si>
+  <si>
+    <t>R1,R2,R7,R8,R14,R15,R16,R17,R18</t>
+  </si>
+  <si>
+    <t>PEC09-2220F-S0012</t>
+  </si>
+  <si>
+    <t>ENC1</t>
+  </si>
+  <si>
+    <t>C14,C15</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>±10% 16V Ceramic Capacitor X7R 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>0604</t>
+  </si>
+  <si>
+    <t>CL05B103KO5NNNC</t>
+  </si>
+  <si>
+    <t>1276-1051-2-ND</t>
+  </si>
+  <si>
+    <t>Rotary Encoder Mechanical 12 Quadrature (Incremental) Right Angle</t>
+  </si>
+  <si>
+    <t>Right Angle</t>
+  </si>
+  <si>
+    <t>Bourns Inc.</t>
+  </si>
+  <si>
+    <t>PEC09-2220F-S0012-ND</t>
   </si>
 </sst>
 </file>
@@ -663,7 +684,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -737,6 +758,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -748,6 +770,18 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Quattrocento Sans"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -937,7 +971,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -981,6 +1015,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1402,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="11.25"/>
@@ -1443,15 +1479,15 @@
         <v>13</v>
       </c>
       <c r="M1" s="6">
-        <f>SUM(M3:M14)</f>
-        <v>10.728</v>
+        <f>SUM(M3:M13)</f>
+        <v>13.568</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
       <c r="O1" s="6">
-        <f>SUM(O3:O14)</f>
-        <v>0.496</v>
+        <f>SUM(O3:O13)</f>
+        <v>5.1111000000000004</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="10.5">
@@ -1533,13 +1569,13 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1549,12 +1585,15 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="8"/>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
       <c r="M5" s="13">
         <v>0</v>
       </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13">
+      <c r="N5" s="19"/>
+      <c r="O5" s="19">
+        <f t="shared" ref="O5:O28" si="0">N5*L5</f>
         <v>0</v>
       </c>
       <c r="P5" s="8"/>
@@ -1571,7 +1610,8 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="11">
-        <v>18</v>
+        <f>A5+1</f>
+        <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>33</v>
@@ -1608,10 +1648,11 @@
         <f>L6*K6</f>
         <v>0.28999999999999998</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="19">
         <v>0.22</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="19">
+        <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
       <c r="P6" s="8"/>
@@ -1627,14 +1668,15 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="11">
-        <v>19</v>
+      <c r="A7" s="17">
+        <f t="shared" ref="A7:A25" si="1">A6+1</f>
+        <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>37</v>
@@ -1664,11 +1706,16 @@
         <v>1</v>
       </c>
       <c r="M7" s="19">
-        <f t="shared" ref="M7:M23" si="0">L7*K7</f>
+        <f t="shared" ref="M7:M22" si="2">L7*K7</f>
         <v>0.44</v>
       </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="N7" s="19">
+        <v>0.33</v>
+      </c>
+      <c r="O7" s="19">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
@@ -1682,14 +1729,15 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="11">
-        <v>20</v>
+      <c r="A8" s="17">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>34</v>
@@ -1719,11 +1767,16 @@
         <v>1</v>
       </c>
       <c r="M8" s="19">
+        <f t="shared" si="2"/>
+        <v>0.24</v>
+      </c>
+      <c r="N8" s="19">
+        <v>0.18</v>
+      </c>
+      <c r="O8" s="19">
         <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+        <v>0.18</v>
+      </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
@@ -1737,14 +1790,15 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="11">
-        <v>24</v>
+      <c r="A9" s="17">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>46</v>
@@ -1774,11 +1828,16 @@
         <v>1</v>
       </c>
       <c r="M9" s="19">
+        <f t="shared" si="2"/>
+        <v>3.47</v>
+      </c>
+      <c r="N9" s="19">
+        <v>2.7078000000000002</v>
+      </c>
+      <c r="O9" s="19">
         <f t="shared" si="0"/>
-        <v>3.47</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+        <v>2.7078000000000002</v>
+      </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
@@ -1792,14 +1851,15 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="11">
-        <v>25</v>
+      <c r="A10" s="17">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>52</v>
@@ -1829,11 +1889,16 @@
         <v>1</v>
       </c>
       <c r="M10" s="19">
+        <f t="shared" si="2"/>
+        <v>1.26</v>
+      </c>
+      <c r="N10" s="19">
+        <v>1.0881000000000001</v>
+      </c>
+      <c r="O10" s="19">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+        <v>1.0881000000000001</v>
+      </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
@@ -1847,14 +1912,15 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="11">
-        <v>26</v>
+      <c r="A11" s="17">
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>57</v>
@@ -1884,11 +1950,16 @@
         <v>1</v>
       </c>
       <c r="M11" s="19">
+        <f t="shared" si="2"/>
+        <v>1.05</v>
+      </c>
+      <c r="N11" s="19">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="O11" s="19">
         <f t="shared" si="0"/>
-        <v>1.05</v>
-      </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+        <v>4.1799999999999997E-2</v>
+      </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -1901,14 +1972,17 @@
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" spans="1:26">
-      <c r="A12" s="11">
-        <v>27</v>
+    <row r="12" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A12" s="17">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="D12" s="12" t="s">
         <v>63</v>
       </c>
@@ -1931,20 +2005,21 @@
         <v>67</v>
       </c>
       <c r="K12" s="13">
-        <v>0.27</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="L12" s="8">
         <v>1</v>
       </c>
       <c r="M12" s="19">
+        <f t="shared" si="2"/>
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="N12" s="19">
+        <v>0.54339999999999999</v>
+      </c>
+      <c r="O12" s="19">
         <f t="shared" si="0"/>
-        <v>0.27</v>
-      </c>
-      <c r="N12" s="13">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="O12" s="13">
-        <v>0.27600000000000002</v>
+        <v>0.54339999999999999</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
@@ -1959,127 +2034,138 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="11">
-        <v>28</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="17">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="H13" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="I13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K13" s="13">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="L13" s="8">
-        <v>1</v>
+      <c r="K13" s="19">
+        <v>3.11</v>
+      </c>
+      <c r="L13" s="15">
+        <v>2</v>
       </c>
       <c r="M13" s="19">
+        <f t="shared" si="2"/>
+        <v>6.22</v>
+      </c>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19">
         <f t="shared" si="0"/>
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="17">
-        <v>56</v>
-      </c>
-      <c r="B14" s="18" t="s">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" s="18" t="s">
+      <c r="C14" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="K14" s="19">
-        <v>3.11</v>
-      </c>
-      <c r="L14" s="15">
-        <v>1</v>
+      <c r="J14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="13">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="L14" s="8">
+        <v>9</v>
       </c>
       <c r="M14" s="19">
+        <f t="shared" si="2"/>
+        <v>5.3100000000000001E-2</v>
+      </c>
+      <c r="N14" s="19">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O14" s="19">
         <f t="shared" si="0"/>
-        <v>3.11</v>
-      </c>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="11">
-        <v>69</v>
+      <c r="A15" s="17">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="12" t="s">
@@ -2089,26 +2175,31 @@
         <v>17</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="K15" s="13">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="L15" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M15" s="19">
+        <f t="shared" si="2"/>
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="N15" s="19">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O15" s="19">
         <f t="shared" si="0"/>
-        <v>2.9499999999999998E-2</v>
-      </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+        <v>2.7199999999999998E-2</v>
+      </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
@@ -2122,17 +2213,18 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="11">
-        <v>71</v>
+      <c r="A16" s="17">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>12</v>
@@ -2144,26 +2236,31 @@
         <v>17</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K16" s="13">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="L16" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M16" s="19">
+        <f t="shared" si="2"/>
+        <v>1.18E-2</v>
+      </c>
+      <c r="N16" s="19">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O16" s="19">
         <f t="shared" si="0"/>
-        <v>3.5400000000000001E-2</v>
-      </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+        <v>1.3599999999999999E-2</v>
+      </c>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
@@ -2177,17 +2274,18 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="11">
-        <v>73</v>
+      <c r="A17" s="17">
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>12</v>
@@ -2199,26 +2297,31 @@
         <v>17</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I17" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K17" s="13">
-        <v>5.8999999999999999E-3</v>
+        <v>8.8999999999999999E-3</v>
       </c>
       <c r="L17" s="8">
         <v>2</v>
       </c>
       <c r="M17" s="19">
+        <f t="shared" si="2"/>
+        <v>1.78E-2</v>
+      </c>
+      <c r="N17" s="19">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O17" s="19">
         <f t="shared" si="0"/>
-        <v>1.18E-2</v>
-      </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
+        <v>1.3599999999999999E-2</v>
+      </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
@@ -2232,17 +2335,18 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="11">
-        <v>74</v>
+      <c r="A18" s="17">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>12</v>
@@ -2251,29 +2355,34 @@
         <v>15</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K18" s="13">
-        <v>8.8999999999999999E-3</v>
+        <v>1.1599999999999999E-2</v>
       </c>
       <c r="L18" s="8">
         <v>2</v>
       </c>
       <c r="M18" s="19">
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="N18" s="19">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="O18" s="19">
         <f t="shared" si="0"/>
-        <v>1.78E-2</v>
-      </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+        <v>2.4400000000000002E-2</v>
+      </c>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
@@ -2287,48 +2396,54 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="11">
-        <v>81</v>
+      <c r="A19" s="17">
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K19" s="13">
-        <v>1.1599999999999999E-2</v>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="L19" s="8">
         <v>1</v>
       </c>
       <c r="M19" s="19">
+        <f t="shared" si="2"/>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="N19" s="19">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="O19" s="19">
         <f t="shared" si="0"/>
-        <v>1.1599999999999999E-2</v>
-      </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+        <v>1.6299999999999999E-2</v>
+      </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
@@ -2342,17 +2457,18 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="11">
-        <v>82</v>
+      <c r="A20" s="17">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>12</v>
@@ -2360,30 +2476,35 @@
       <c r="F20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>101</v>
+      <c r="G20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="12" t="s">
-        <v>102</v>
+      <c r="J20" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="K20" s="13">
-        <v>1.5599999999999999E-2</v>
+        <v>3.3099999999999997E-2</v>
       </c>
       <c r="L20" s="8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M20" s="19">
+        <f t="shared" si="2"/>
+        <v>0.1986</v>
+      </c>
+      <c r="N20" s="19">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="O20" s="19">
         <f t="shared" si="0"/>
-        <v>1.5599999999999999E-2</v>
-      </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+        <v>0.20579999999999998</v>
+      </c>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
@@ -2397,17 +2518,18 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26">
-      <c r="A21" s="11">
-        <v>83</v>
+      <c r="A21" s="17">
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>104</v>
+        <v>119</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>12</v>
@@ -2415,30 +2537,35 @@
       <c r="F21" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>105</v>
+      <c r="G21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>106</v>
+      <c r="J21" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="K21" s="13">
-        <v>3.3099999999999997E-2</v>
+        <v>0.1</v>
       </c>
       <c r="L21" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M21" s="19">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="N21" s="19">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="O21" s="19">
         <f t="shared" si="0"/>
-        <v>0.1986</v>
-      </c>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+        <v>1.8499999999999999E-2</v>
+      </c>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
@@ -2452,19 +2579,20 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="11">
-        <v>84</v>
+      <c r="A22" s="17">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="12" t="s">
@@ -2474,29 +2602,30 @@
         <v>16</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="I22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="K22" s="13">
-        <v>0.1</v>
+        <v>3.1600000000000003E-2</v>
       </c>
       <c r="L22" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M22" s="19">
+        <f t="shared" si="2"/>
+        <v>6.3200000000000006E-2</v>
+      </c>
+      <c r="N22" s="19">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="O22" s="19">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="N22" s="13">
-        <v>1.8499999999999999E-2</v>
-      </c>
-      <c r="O22" s="13">
-        <v>1.8499999999999999E-2</v>
+        <v>6.6199999999999995E-2</v>
       </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
@@ -2511,19 +2640,20 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="11">
-        <v>85</v>
+      <c r="A23" s="17">
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="12" t="s">
@@ -2533,26 +2663,31 @@
         <v>16</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I23" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K23" s="13">
-        <v>3.1600000000000003E-2</v>
+        <v>6.7199999999999996E-2</v>
       </c>
       <c r="L23" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M23" s="19">
+        <f>L23*K23</f>
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="N23" s="19">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="O23" s="19">
         <f t="shared" si="0"/>
-        <v>9.4800000000000009E-2</v>
-      </c>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
+        <v>6.8400000000000002E-2</v>
+      </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
@@ -2565,148 +2700,218 @@
       <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24" spans="1:26">
-      <c r="A24" s="11">
-        <v>88</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" s="12" t="s">
+    <row r="24" spans="1:26" ht="12">
+      <c r="A24" s="17">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="12" t="s">
+      <c r="F24" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="12" t="s">
+      <c r="H24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="K24" s="13">
-        <v>6.7199999999999996E-2</v>
-      </c>
-      <c r="L24" s="8">
+      <c r="J24" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="L24" s="1">
+        <v>2</v>
+      </c>
+      <c r="M24" s="1">
+        <f>L24*K24</f>
+        <v>0.2</v>
+      </c>
+      <c r="N24" s="23">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="O24" s="19">
+        <f t="shared" si="0"/>
+        <v>1.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25" s="17">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K25" s="1">
+        <v>3.16</v>
+      </c>
+      <c r="L25" s="1">
         <v>1</v>
       </c>
-      <c r="M24" s="19">
-        <f>L24*K24</f>
-        <v>6.7199999999999996E-2</v>
-      </c>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="8"/>
+      <c r="M25" s="1">
+        <f>L25*K25</f>
+        <v>3.16</v>
+      </c>
+      <c r="N25" s="23">
+        <v>2.1499000000000001</v>
+      </c>
+      <c r="O25" s="19">
+        <f t="shared" si="0"/>
+        <v>2.1499000000000001</v>
+      </c>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="17">
+      <c r="N27" s="23"/>
+      <c r="O27" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="A29" s="17">
+        <v>22</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="K29" s="19">
+        <v>2.68</v>
+      </c>
+      <c r="L29" s="15">
         <v>1</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="K27" s="19">
+      <c r="M29" s="19">
+        <f>L29*K29</f>
         <v>2.68</v>
       </c>
-      <c r="L27" s="15">
-        <v>1</v>
-      </c>
-      <c r="M27" s="19">
-        <f>L27*K27</f>
-        <v>2.68</v>
-      </c>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
+      <c r="N29" s="19">
+        <v>1.82</v>
+      </c>
+      <c r="O29" s="19">
+        <f>N29*L29</f>
+        <v>1.82</v>
+      </c>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="15"/>
+      <c r="Z29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Encoder changed, BOMs updated
</commit_message>
<xml_diff>
--- a/Hardware/Extra/Bottom/Smartwatch-EXTRA-BOTTOM_BOM.xlsx
+++ b/Hardware/Extra/Bottom/Smartwatch-EXTRA-BOTTOM_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruhaan Joshi\Documents\Smartwatch\Hardware\Extra\Bottom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC45444-EF69-4D2C-AD21-16C79BE40AC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD587E4-C247-488F-81FC-A11B03F090F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7635" yWindow="3705" windowWidth="14400" windowHeight="11340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="152">
   <si>
     <t>BOM #</t>
   </si>
@@ -625,9 +625,6 @@
     <t>R1,R2,R7,R8,R14,R15,R16,R17,R18</t>
   </si>
   <si>
-    <t>PEC09-2220F-S0012</t>
-  </si>
-  <si>
     <t>ENC1</t>
   </si>
   <si>
@@ -649,18 +646,6 @@
     <t>1276-1051-2-ND</t>
   </si>
   <si>
-    <t>Rotary Encoder Mechanical 12 Quadrature (Incremental) Right Angle</t>
-  </si>
-  <si>
-    <t>Right Angle</t>
-  </si>
-  <si>
-    <t>Bourns Inc.</t>
-  </si>
-  <si>
-    <t>PEC09-2220F-S0012-ND</t>
-  </si>
-  <si>
     <t>CONN_07-1.27MM (CONN_07)</t>
   </si>
   <si>
@@ -674,6 +659,39 @@
   </si>
   <si>
     <t>J1,J2</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>Tactile Button</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>Rotary Encoder Mechanical 12 Quadrature (Incremental) Vertical</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>EVQ-VUA00112B</t>
+  </si>
+  <si>
+    <t>P123413-ND</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 1VA 32V</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>KT11P2SA1M35LFG</t>
+  </si>
+  <si>
+    <t>CKN1843CT-ND</t>
   </si>
 </sst>
 </file>
@@ -977,7 +995,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1014,6 +1032,12 @@
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="82" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="83" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="83" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="83" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="83" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1023,12 +1047,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="83" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="83" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="83" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="83" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="84">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1451,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="11.25"/>
@@ -1475,12 +1494,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="3" customFormat="1" ht="14.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -1606,7 +1625,7 @@
       </c>
       <c r="N5" s="19"/>
       <c r="O5" s="19">
-        <f t="shared" ref="O5:O28" si="0">N5*L5</f>
+        <f t="shared" ref="O5:O27" si="0">N5*L5</f>
         <v>0</v>
       </c>
       <c r="P5" s="8"/>
@@ -1682,7 +1701,7 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="17">
-        <f t="shared" ref="A7:A25" si="1">A6+1</f>
+        <f t="shared" ref="A7:A26" si="1">A6+1</f>
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1719,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="19">
-        <f t="shared" ref="M7:M25" si="2">L7*K7</f>
+        <f t="shared" ref="M7:M26" si="2">L7*K7</f>
         <v>0.44</v>
       </c>
       <c r="N7" s="19">
@@ -1872,7 +1891,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>52</v>
@@ -2047,57 +2066,57 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="26">
+      <c r="A13" s="23">
         <v>55</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="27" t="s">
+      <c r="B13" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="27" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="I13" s="27" t="s">
+      <c r="H13" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="K13" s="28">
+      <c r="J13" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="K13" s="25">
         <v>5.0599999999999996</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="22">
         <v>1</v>
       </c>
       <c r="M13" s="19">
         <f t="shared" si="2"/>
         <v>5.0599999999999996</v>
       </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="22"/>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="17">
@@ -2718,33 +2737,33 @@
         <v>127</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="K24" s="1">
+        <v>135</v>
+      </c>
+      <c r="K24" s="20">
         <v>0.1</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L24" s="29">
         <v>2</v>
       </c>
       <c r="M24" s="19">
@@ -2765,84 +2784,174 @@
         <v>67</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="K25" s="1">
-        <v>3.16</v>
-      </c>
-      <c r="L25" s="1">
+        <v>147</v>
+      </c>
+      <c r="K25" s="20">
+        <v>1.18</v>
+      </c>
+      <c r="L25" s="29">
         <v>1</v>
       </c>
-      <c r="M25" s="19">
+      <c r="M25" s="20">
         <f t="shared" si="2"/>
-        <v>3.16</v>
+        <v>1.18</v>
       </c>
       <c r="N25" s="20">
-        <v>2.1499000000000001</v>
+        <v>0.80625000000000002</v>
       </c>
       <c r="O25" s="19">
         <f t="shared" si="0"/>
-        <v>2.1499000000000001</v>
+        <v>0.80625000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:26">
-      <c r="N26" s="20"/>
+      <c r="A26" s="17">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K26" s="20">
+        <v>4.47</v>
+      </c>
+      <c r="L26" s="29">
+        <v>1</v>
+      </c>
+      <c r="M26" s="20">
+        <f t="shared" si="2"/>
+        <v>4.47</v>
+      </c>
+      <c r="N26" s="20">
+        <v>3.3904000000000001</v>
+      </c>
       <c r="O26" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.3904000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:26">
-      <c r="N27" s="20"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="19"/>
       <c r="O27" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="15"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16" t="s">
+      <c r="A28" s="17">
+        <v>22</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="19"/>
+      <c r="J28" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="K28" s="19">
+        <v>2.68</v>
+      </c>
+      <c r="L28" s="15">
+        <v>1</v>
+      </c>
+      <c r="M28" s="19">
+        <f>L28*K28</f>
+        <v>2.68</v>
+      </c>
+      <c r="N28" s="19">
+        <v>1.82</v>
+      </c>
       <c r="O28" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>N28*L28</f>
+        <v>1.82</v>
       </c>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
@@ -2856,73 +2965,13 @@
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
     </row>
-    <row r="29" spans="1:26">
-      <c r="A29" s="17">
-        <v>22</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="K29" s="19">
-        <v>2.68</v>
-      </c>
-      <c r="L29" s="15">
-        <v>1</v>
-      </c>
-      <c r="M29" s="19">
-        <f>L29*K29</f>
-        <v>2.68</v>
-      </c>
-      <c r="N29" s="19">
-        <v>1.82</v>
-      </c>
-      <c r="O29" s="19">
-        <f>N29*L29</f>
-        <v>1.82</v>
-      </c>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="15"/>
-      <c r="Z29" s="15"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>